<commit_message>
Creación función 1 y 2, con sus interfaces
</commit_message>
<xml_diff>
--- a/Main (no listo)/sedes.xlsx
+++ b/Main (no listo)/sedes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Estudios de Ale\Compu\GitHub\Tareas Programadas\TareaProgramada2\TareaProgramada2\Main (no listo)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FE718B3-FD4B-435E-BF5A-9F8FA3DF9FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0119229-F8FB-4A11-885D-2EE5D76D8321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3135" yWindow="1215" windowWidth="21600" windowHeight="11385" xr2:uid="{E0B51441-81EE-421A-8369-62DB6E03DD2B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E0B51441-81EE-421A-8369-62DB6E03DD2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,21 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
-    <t xml:space="preserve">Campus Tecnológico de San Carlos </t>
-  </si>
-  <si>
-    <t>Campus Tecnológico de San José</t>
-  </si>
-  <si>
-    <t>Centro Académico Limón</t>
-  </si>
-  <si>
-    <t>Campus Tecnológico Central de Cartago</t>
-  </si>
-  <si>
-    <t>Centro Académico de Alajuela</t>
-  </si>
-  <si>
     <t>Bachillerato en Administración de Empresas</t>
   </si>
   <si>
@@ -126,14 +111,37 @@
   </si>
   <si>
     <t>Licenciatura en Mantenimiento Industrial</t>
+  </si>
+  <si>
+    <t>CAMPUS TECNOLÓGICO LOCAL SAN CARLOS</t>
+  </si>
+  <si>
+    <t>CAMPUS TECNOLÓGICO LOCAL SAN JOSÉ</t>
+  </si>
+  <si>
+    <t>CENTRO ACADÉMICO DE LIMÓN</t>
+  </si>
+  <si>
+    <t>CAMPUS TECNOLÓGICO CENTRAL CARTAGO</t>
+  </si>
+  <si>
+    <t>CENTRO ACADÉMICO DE ALAJUELA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -163,7 +171,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,9 +488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{761FF26A-DADC-4CDF-83CE-AA13D2015D92}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -494,164 +500,165 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="1" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="1" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D9" s="1" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D11" s="1" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D12" s="1" t="s">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D13" s="1" t="s">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D14" s="1" t="s">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="1"/>
+      <c r="D20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="1" t="s">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D16" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D17" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D18" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D19" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D20" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D21" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Opción 2 con errores
</commit_message>
<xml_diff>
--- a/Main (no listo)/sedes.xlsx
+++ b/Main (no listo)/sedes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Estudios de Ale\Compu\GitHub\Tareas Programadas\TareaProgramada2\TareaProgramada2\Main (no listo)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0119229-F8FB-4A11-885D-2EE5D76D8321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B659E89C-E1B8-4566-9329-F212079D75E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E0B51441-81EE-421A-8369-62DB6E03DD2B}"/>
   </bookViews>
@@ -488,7 +488,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{761FF26A-DADC-4CDF-83CE-AA13D2015D92}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>